<commit_message>
Fix a bug when deleting
</commit_message>
<xml_diff>
--- a/Documentation/Linked Historians QA.xlsx
+++ b/Documentation/Linked Historians QA.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10FF4391-6A86-462E-94D0-BEB9B887B6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bombt\Desktop\proekt\linked-list-sprint-project-linked-historians\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFC7541-CA8A-4D14-8444-BF7DA9920DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>LINKED HISTORIANS</t>
   </si>
@@ -181,13 +186,16 @@
   </si>
   <si>
     <t>Sends the user back to the main menu from where they can either add an event, open the list with events from the local database or get back to the authentication menu</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -410,27 +418,46 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,25 +476,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
@@ -555,9 +563,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -595,7 +603,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -701,7 +709,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -843,7 +851,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,283 +862,283 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
-    <col min="5" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" ht="18">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5" t="s">
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:4" ht="30.75">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" ht="30.75">
-      <c r="A7" s="4" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" ht="45.75">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30.75">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30.75">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="11" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" ht="30.75">
-      <c r="A13" s="4" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="30.75">
-      <c r="A14" s="4" t="s">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45.75">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" ht="60.75">
-      <c r="A16" s="4" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="14" t="s">
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30.75">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45.75">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="30.75">
-      <c r="A19" s="4" t="s">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" ht="45.75">
-      <c r="A20" s="4" t="s">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="16"/>
-    </row>
-    <row r="22" spans="1:4" ht="60.75">
-      <c r="A22" s="17" t="s">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="20"/>
+      <c r="D22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>